<commit_message>
commit 18 - first half
</commit_message>
<xml_diff>
--- a/Infra details.xlsx
+++ b/Infra details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\AWS\Sunbird cdk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDC3812-2835-436D-BC30-3A1453ABA3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51F0002-F1DA-4D57-8096-759A2209902D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="8580" yWindow="3520" windowWidth="7500" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Sr.No</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Default will be taken by RDS</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -249,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -283,6 +286,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,15 +575,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="4"/>
     <col min="2" max="2" width="41.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.453125" style="5" customWidth="1"/>
     <col min="5" max="5" width="25.7265625" style="5" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="4"/>
@@ -836,16 +845,16 @@
       <c r="A23" s="11">
         <v>21</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="5" t="s">
+      <c r="C23" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="13" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>